<commit_message>
LSTM serieal 2 ran
</commit_message>
<xml_diff>
--- a/LSTM/lstm_info.xlsx
+++ b/LSTM/lstm_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>serial</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>accuracy</t>
+  </si>
+  <si>
+    <t>50 epoch 이상 과적합</t>
   </si>
 </sst>
 </file>
@@ -42,13 +45,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -89,20 +98,20 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -415,7 +424,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -425,12 +434,13 @@
     <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="8" width="16.433571428571426" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="19.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,69 +453,92 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>100</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="4">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>10</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>128</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>10</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="6">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
+      <c r="B3" s="5">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4">
+        <v>128</v>
+      </c>
+      <c r="F3" s="5">
+        <v>20</v>
+      </c>
+      <c r="G3" s="6">
+        <v>78</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="6">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>